<commit_message>
end of data collection
</commit_message>
<xml_diff>
--- a/RFID Index.xlsx
+++ b/RFID Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\PycharmProjects\RFID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E415EC6-AF1D-464C-8745-8FAA6E1EEF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC1D6A1-10D8-48DC-B11F-93AD13DE0659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>ציוד</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>71, 72</t>
+  </si>
+  <si>
+    <t>81,..85</t>
+  </si>
+  <si>
+    <t>91,…95</t>
   </si>
 </sst>
 </file>
@@ -696,7 +702,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1144,9 @@
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1188,7 +1196,9 @@
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1999,7 +2009,7 @@
         <v>21</v>
       </c>
       <c r="D27" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="8"/>
@@ -2018,9 +2028,7 @@
         <v>30</v>
       </c>
       <c r="I27" s="12"/>
-      <c r="J27" s="1">
-        <v>2</v>
-      </c>
+      <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="2"/>

</xml_diff>